<commit_message>
Changes after finishing the course
</commit_message>
<xml_diff>
--- a/Python Project/country_codes.xlsx
+++ b/Python Project/country_codes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jlowh\Documents\DSE5002\Python Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sue_susman/Desktop/Data Science Files/DSE 5002 R &amp; Python Programming/GitHub/DSE5002/Python Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9C9BD94A-49B0-46D2-9EEA-B110CB72AFBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46167FF6-AB82-8445-B785-3D89D70397CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{1F197760-E0EE-4CE5-9893-1B6F4636E5D2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20740" windowHeight="11040" xr2:uid="{1F197760-E0EE-4CE5-9893-1B6F4636E5D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2737,17 +2737,16 @@
   <dimension ref="A1:D250"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="29.33203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" customWidth="1"/>
-    <col min="2" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="48" thickBot="1">
+    <row r="1" spans="1:4" ht="35" thickBot="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2761,7 +2760,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30.75" thickBot="1">
+    <row r="2" spans="1:4" ht="18" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -2775,7 +2774,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.75" thickBot="1">
+    <row r="3" spans="1:4" ht="18" thickBot="1">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -2789,7 +2788,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" thickBot="1">
+    <row r="4" spans="1:4" ht="18" thickBot="1">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -2803,7 +2802,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="45.75" thickBot="1">
+    <row r="5" spans="1:4" ht="18" thickBot="1">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -2817,7 +2816,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="30.75" thickBot="1">
+    <row r="6" spans="1:4" ht="18" thickBot="1">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
@@ -2831,7 +2830,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.75" thickBot="1">
+    <row r="7" spans="1:4" ht="18" thickBot="1">
       <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
@@ -2845,7 +2844,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.75" thickBot="1">
+    <row r="8" spans="1:4" ht="18" thickBot="1">
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
@@ -2859,7 +2858,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="30.75" thickBot="1">
+    <row r="9" spans="1:4" ht="18" thickBot="1">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
@@ -2873,7 +2872,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="60.75" thickBot="1">
+    <row r="10" spans="1:4" ht="35" thickBot="1">
       <c r="A10" s="1" t="s">
         <v>28</v>
       </c>
@@ -2887,7 +2886,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="30.75" thickBot="1">
+    <row r="11" spans="1:4" ht="18" thickBot="1">
       <c r="A11" s="1" t="s">
         <v>31</v>
       </c>
@@ -2901,7 +2900,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="30.75" thickBot="1">
+    <row r="12" spans="1:4" ht="18" thickBot="1">
       <c r="A12" s="1" t="s">
         <v>34</v>
       </c>
@@ -2915,7 +2914,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.75" thickBot="1">
+    <row r="13" spans="1:4" ht="18" thickBot="1">
       <c r="A13" s="1" t="s">
         <v>37</v>
       </c>
@@ -2929,7 +2928,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="30.75" thickBot="1">
+    <row r="14" spans="1:4" ht="18" thickBot="1">
       <c r="A14" s="1" t="s">
         <v>40</v>
       </c>
@@ -2943,7 +2942,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15.75" thickBot="1">
+    <row r="15" spans="1:4" ht="18" thickBot="1">
       <c r="A15" s="1" t="s">
         <v>43</v>
       </c>
@@ -2957,7 +2956,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="30.75" thickBot="1">
+    <row r="16" spans="1:4" ht="18" thickBot="1">
       <c r="A16" s="1" t="s">
         <v>46</v>
       </c>
@@ -2971,7 +2970,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="30.75" thickBot="1">
+    <row r="17" spans="1:4" ht="18" thickBot="1">
       <c r="A17" s="1" t="s">
         <v>49</v>
       </c>
@@ -2985,7 +2984,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.75" thickBot="1">
+    <row r="18" spans="1:4" ht="18" thickBot="1">
       <c r="A18" s="1" t="s">
         <v>52</v>
       </c>
@@ -2999,7 +2998,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="30.75" thickBot="1">
+    <row r="19" spans="1:4" ht="18" thickBot="1">
       <c r="A19" s="1" t="s">
         <v>55</v>
       </c>
@@ -3013,7 +3012,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="30.75" thickBot="1">
+    <row r="20" spans="1:4" ht="18" thickBot="1">
       <c r="A20" s="1" t="s">
         <v>58</v>
       </c>
@@ -3027,7 +3026,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15.75" thickBot="1">
+    <row r="21" spans="1:4" ht="18" thickBot="1">
       <c r="A21" s="1" t="s">
         <v>61</v>
       </c>
@@ -3041,7 +3040,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="30.75" thickBot="1">
+    <row r="22" spans="1:4" ht="18" thickBot="1">
       <c r="A22" s="1" t="s">
         <v>64</v>
       </c>
@@ -3055,7 +3054,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15.75" thickBot="1">
+    <row r="23" spans="1:4" ht="18" thickBot="1">
       <c r="A23" s="1" t="s">
         <v>67</v>
       </c>
@@ -3069,7 +3068,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15.75" thickBot="1">
+    <row r="24" spans="1:4" ht="18" thickBot="1">
       <c r="A24" s="1" t="s">
         <v>70</v>
       </c>
@@ -3083,7 +3082,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="30.75" thickBot="1">
+    <row r="25" spans="1:4" ht="18" thickBot="1">
       <c r="A25" s="1" t="s">
         <v>73</v>
       </c>
@@ -3097,7 +3096,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15.75" thickBot="1">
+    <row r="26" spans="1:4" ht="18" thickBot="1">
       <c r="A26" s="1" t="s">
         <v>76</v>
       </c>
@@ -3111,7 +3110,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="75.75" thickBot="1">
+    <row r="27" spans="1:4" ht="52" thickBot="1">
       <c r="A27" s="1" t="s">
         <v>79</v>
       </c>
@@ -3125,7 +3124,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="75.75" thickBot="1">
+    <row r="28" spans="1:4" ht="52" thickBot="1">
       <c r="A28" s="1" t="s">
         <v>82</v>
       </c>
@@ -3139,7 +3138,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="60.75" thickBot="1">
+    <row r="29" spans="1:4" ht="35" thickBot="1">
       <c r="A29" s="1" t="s">
         <v>85</v>
       </c>
@@ -3153,7 +3152,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="30.75" thickBot="1">
+    <row r="30" spans="1:4" ht="18" thickBot="1">
       <c r="A30" s="1" t="s">
         <v>88</v>
       </c>
@@ -3167,7 +3166,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="30.75" thickBot="1">
+    <row r="31" spans="1:4" ht="18" thickBot="1">
       <c r="A31" s="1" t="s">
         <v>91</v>
       </c>
@@ -3181,7 +3180,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15.75" thickBot="1">
+    <row r="32" spans="1:4" ht="18" thickBot="1">
       <c r="A32" s="1" t="s">
         <v>94</v>
       </c>
@@ -3195,7 +3194,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="75.75" thickBot="1">
+    <row r="33" spans="1:4" ht="52" thickBot="1">
       <c r="A33" s="1" t="s">
         <v>97</v>
       </c>
@@ -3209,7 +3208,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="45.75" thickBot="1">
+    <row r="34" spans="1:4" ht="35" thickBot="1">
       <c r="A34" s="1" t="s">
         <v>100</v>
       </c>
@@ -3223,7 +3222,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="30.75" thickBot="1">
+    <row r="35" spans="1:4" ht="18" thickBot="1">
       <c r="A35" s="1" t="s">
         <v>103</v>
       </c>
@@ -3237,7 +3236,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="30.75" thickBot="1">
+    <row r="36" spans="1:4" ht="18" thickBot="1">
       <c r="A36" s="1" t="s">
         <v>106</v>
       </c>
@@ -3251,7 +3250,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15.75" thickBot="1">
+    <row r="37" spans="1:4" ht="18" thickBot="1">
       <c r="A37" s="1" t="s">
         <v>109</v>
       </c>
@@ -3265,7 +3264,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="30.75" thickBot="1">
+    <row r="38" spans="1:4" ht="18" thickBot="1">
       <c r="A38" s="1" t="s">
         <v>112</v>
       </c>
@@ -3279,7 +3278,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="30.75" thickBot="1">
+    <row r="39" spans="1:4" ht="18" thickBot="1">
       <c r="A39" s="1" t="s">
         <v>115</v>
       </c>
@@ -3293,7 +3292,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="30.75" thickBot="1">
+    <row r="40" spans="1:4" ht="18" thickBot="1">
       <c r="A40" s="1" t="s">
         <v>118</v>
       </c>
@@ -3307,7 +3306,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="30.75" thickBot="1">
+    <row r="41" spans="1:4" ht="18" thickBot="1">
       <c r="A41" s="1" t="s">
         <v>121</v>
       </c>
@@ -3321,7 +3320,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="60.75" thickBot="1">
+    <row r="42" spans="1:4" ht="35" thickBot="1">
       <c r="A42" s="1" t="s">
         <v>124</v>
       </c>
@@ -3335,7 +3334,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="60.75" thickBot="1">
+    <row r="43" spans="1:4" ht="35" thickBot="1">
       <c r="A43" s="1" t="s">
         <v>127</v>
       </c>
@@ -3349,7 +3348,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="15.75" thickBot="1">
+    <row r="44" spans="1:4" ht="18" thickBot="1">
       <c r="A44" s="1" t="s">
         <v>130</v>
       </c>
@@ -3363,7 +3362,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="15.75" thickBot="1">
+    <row r="45" spans="1:4" ht="18" thickBot="1">
       <c r="A45" s="1" t="s">
         <v>133</v>
       </c>
@@ -3377,7 +3376,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="15.75" thickBot="1">
+    <row r="46" spans="1:4" ht="18" thickBot="1">
       <c r="A46" s="1" t="s">
         <v>136</v>
       </c>
@@ -3391,7 +3390,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="45.75" thickBot="1">
+    <row r="47" spans="1:4" ht="18" thickBot="1">
       <c r="A47" s="1" t="s">
         <v>139</v>
       </c>
@@ -3405,7 +3404,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="75.75" thickBot="1">
+    <row r="48" spans="1:4" ht="35" thickBot="1">
       <c r="A48" s="1" t="s">
         <v>142</v>
       </c>
@@ -3419,7 +3418,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="30.75" thickBot="1">
+    <row r="49" spans="1:4" ht="18" thickBot="1">
       <c r="A49" s="1" t="s">
         <v>145</v>
       </c>
@@ -3433,7 +3432,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="30.75" thickBot="1">
+    <row r="50" spans="1:4" ht="18" thickBot="1">
       <c r="A50" s="1" t="s">
         <v>148</v>
       </c>
@@ -3447,7 +3446,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="90.75" thickBot="1">
+    <row r="51" spans="1:4" ht="52" thickBot="1">
       <c r="A51" s="1" t="s">
         <v>151</v>
       </c>
@@ -3461,7 +3460,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="30.75" thickBot="1">
+    <row r="52" spans="1:4" ht="18" thickBot="1">
       <c r="A52" s="1" t="s">
         <v>154</v>
       </c>
@@ -3475,7 +3474,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="45.75" thickBot="1">
+    <row r="53" spans="1:4" ht="35" thickBot="1">
       <c r="A53" s="1" t="s">
         <v>157</v>
       </c>
@@ -3489,7 +3488,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="30.75" thickBot="1">
+    <row r="54" spans="1:4" ht="18" thickBot="1">
       <c r="A54" s="1" t="s">
         <v>160</v>
       </c>
@@ -3503,7 +3502,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="15.75" thickBot="1">
+    <row r="55" spans="1:4" ht="18" thickBot="1">
       <c r="A55" s="1" t="s">
         <v>163</v>
       </c>
@@ -3517,7 +3516,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="15.75" thickBot="1">
+    <row r="56" spans="1:4" ht="18" thickBot="1">
       <c r="A56" s="1" t="s">
         <v>166</v>
       </c>
@@ -3531,7 +3530,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="30.75" thickBot="1">
+    <row r="57" spans="1:4" ht="18" thickBot="1">
       <c r="A57" s="1" t="s">
         <v>169</v>
       </c>
@@ -3545,7 +3544,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="15.75" thickBot="1">
+    <row r="58" spans="1:4" ht="18" thickBot="1">
       <c r="A58" s="1" t="s">
         <v>172</v>
       </c>
@@ -3559,7 +3558,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="30.75" thickBot="1">
+    <row r="59" spans="1:4" ht="18" thickBot="1">
       <c r="A59" s="1" t="s">
         <v>175</v>
       </c>
@@ -3573,7 +3572,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="30.75" thickBot="1">
+    <row r="60" spans="1:4" ht="18" thickBot="1">
       <c r="A60" s="1" t="s">
         <v>178</v>
       </c>
@@ -3587,7 +3586,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="30.75" thickBot="1">
+    <row r="61" spans="1:4" ht="18" thickBot="1">
       <c r="A61" s="1" t="s">
         <v>181</v>
       </c>
@@ -3601,7 +3600,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="15.75" thickBot="1">
+    <row r="62" spans="1:4" ht="18" thickBot="1">
       <c r="A62" s="1" t="s">
         <v>184</v>
       </c>
@@ -3615,7 +3614,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="30.75" thickBot="1">
+    <row r="63" spans="1:4" ht="18" thickBot="1">
       <c r="A63" s="1" t="s">
         <v>187</v>
       </c>
@@ -3629,7 +3628,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="60.75" thickBot="1">
+    <row r="64" spans="1:4" ht="35" thickBot="1">
       <c r="A64" s="1" t="s">
         <v>190</v>
       </c>
@@ -3643,7 +3642,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="30.75" thickBot="1">
+    <row r="65" spans="1:4" ht="18" thickBot="1">
       <c r="A65" s="1" t="s">
         <v>193</v>
       </c>
@@ -3657,7 +3656,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="15.75" thickBot="1">
+    <row r="66" spans="1:4" ht="18" thickBot="1">
       <c r="A66" s="1" t="s">
         <v>196</v>
       </c>
@@ -3671,7 +3670,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="45.75" thickBot="1">
+    <row r="67" spans="1:4" ht="18" thickBot="1">
       <c r="A67" s="1" t="s">
         <v>199</v>
       </c>
@@ -3685,7 +3684,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="45.75" thickBot="1">
+    <row r="68" spans="1:4" ht="35" thickBot="1">
       <c r="A68" s="1" t="s">
         <v>202</v>
       </c>
@@ -3699,7 +3698,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="15.75" thickBot="1">
+    <row r="69" spans="1:4" ht="18" thickBot="1">
       <c r="A69" s="1" t="s">
         <v>205</v>
       </c>
@@ -3713,7 +3712,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="15.75" thickBot="1">
+    <row r="70" spans="1:4" ht="18" thickBot="1">
       <c r="A70" s="1" t="s">
         <v>208</v>
       </c>
@@ -3727,7 +3726,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="30.75" thickBot="1">
+    <row r="71" spans="1:4" ht="18" thickBot="1">
       <c r="A71" s="1" t="s">
         <v>211</v>
       </c>
@@ -3741,7 +3740,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="30.75" thickBot="1">
+    <row r="72" spans="1:4" ht="18" thickBot="1">
       <c r="A72" s="1" t="s">
         <v>214</v>
       </c>
@@ -3755,7 +3754,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="90.75" thickBot="1">
+    <row r="73" spans="1:4" ht="35" thickBot="1">
       <c r="A73" s="1" t="s">
         <v>217</v>
       </c>
@@ -3769,7 +3768,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="45.75" thickBot="1">
+    <row r="74" spans="1:4" ht="35" thickBot="1">
       <c r="A74" s="1" t="s">
         <v>220</v>
       </c>
@@ -3783,7 +3782,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="15.75" thickBot="1">
+    <row r="75" spans="1:4" ht="18" thickBot="1">
       <c r="A75" s="1" t="s">
         <v>223</v>
       </c>
@@ -3797,7 +3796,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="15.75" thickBot="1">
+    <row r="76" spans="1:4" ht="18" thickBot="1">
       <c r="A76" s="1" t="s">
         <v>226</v>
       </c>
@@ -3811,7 +3810,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="15.75" thickBot="1">
+    <row r="77" spans="1:4" ht="18" thickBot="1">
       <c r="A77" s="1" t="s">
         <v>229</v>
       </c>
@@ -3825,7 +3824,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="30.75" thickBot="1">
+    <row r="78" spans="1:4" ht="18" thickBot="1">
       <c r="A78" s="1" t="s">
         <v>232</v>
       </c>
@@ -3839,7 +3838,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="45.75" thickBot="1">
+    <row r="79" spans="1:4" ht="18" thickBot="1">
       <c r="A79" s="1" t="s">
         <v>235</v>
       </c>
@@ -3853,7 +3852,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="75.75" thickBot="1">
+    <row r="80" spans="1:4" ht="35" thickBot="1">
       <c r="A80" s="1" t="s">
         <v>238</v>
       </c>
@@ -3867,7 +3866,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="15.75" thickBot="1">
+    <row r="81" spans="1:4" ht="18" thickBot="1">
       <c r="A81" s="1" t="s">
         <v>241</v>
       </c>
@@ -3881,7 +3880,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="30.75" thickBot="1">
+    <row r="82" spans="1:4" ht="18" thickBot="1">
       <c r="A82" s="1" t="s">
         <v>244</v>
       </c>
@@ -3895,7 +3894,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="30.75" thickBot="1">
+    <row r="83" spans="1:4" ht="18" thickBot="1">
       <c r="A83" s="1" t="s">
         <v>247</v>
       </c>
@@ -3909,7 +3908,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="30.75" thickBot="1">
+    <row r="84" spans="1:4" ht="18" thickBot="1">
       <c r="A84" s="1" t="s">
         <v>250</v>
       </c>
@@ -3923,7 +3922,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="15.75" thickBot="1">
+    <row r="85" spans="1:4" ht="18" thickBot="1">
       <c r="A85" s="1" t="s">
         <v>253</v>
       </c>
@@ -3937,7 +3936,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="30.75" thickBot="1">
+    <row r="86" spans="1:4" ht="18" thickBot="1">
       <c r="A86" s="1" t="s">
         <v>256</v>
       </c>
@@ -3951,7 +3950,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="15.75" thickBot="1">
+    <row r="87" spans="1:4" ht="18" thickBot="1">
       <c r="A87" s="1" t="s">
         <v>259</v>
       </c>
@@ -3965,7 +3964,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="30.75" thickBot="1">
+    <row r="88" spans="1:4" ht="18" thickBot="1">
       <c r="A88" s="1" t="s">
         <v>262</v>
       </c>
@@ -3979,7 +3978,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="30.75" thickBot="1">
+    <row r="89" spans="1:4" ht="18" thickBot="1">
       <c r="A89" s="1" t="s">
         <v>265</v>
       </c>
@@ -3993,7 +3992,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="30.75" thickBot="1">
+    <row r="90" spans="1:4" ht="18" thickBot="1">
       <c r="A90" s="1" t="s">
         <v>268</v>
       </c>
@@ -4007,7 +4006,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="15.75" thickBot="1">
+    <row r="91" spans="1:4" ht="18" thickBot="1">
       <c r="A91" s="1" t="s">
         <v>271</v>
       </c>
@@ -4021,7 +4020,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="30.75" thickBot="1">
+    <row r="92" spans="1:4" ht="18" thickBot="1">
       <c r="A92" s="1" t="s">
         <v>274</v>
       </c>
@@ -4035,7 +4034,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="30.75" thickBot="1">
+    <row r="93" spans="1:4" ht="18" thickBot="1">
       <c r="A93" s="1" t="s">
         <v>277</v>
       </c>
@@ -4049,7 +4048,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="15.75" thickBot="1">
+    <row r="94" spans="1:4" ht="18" thickBot="1">
       <c r="A94" s="1" t="s">
         <v>280</v>
       </c>
@@ -4063,7 +4062,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="30.75" thickBot="1">
+    <row r="95" spans="1:4" ht="18" thickBot="1">
       <c r="A95" s="1" t="s">
         <v>283</v>
       </c>
@@ -4077,7 +4076,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="15.75" thickBot="1">
+    <row r="96" spans="1:4" ht="18" thickBot="1">
       <c r="A96" s="1" t="s">
         <v>286</v>
       </c>
@@ -4091,7 +4090,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="15.75" thickBot="1">
+    <row r="97" spans="1:4" ht="18" thickBot="1">
       <c r="A97" s="1" t="s">
         <v>289</v>
       </c>
@@ -4105,7 +4104,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="98" spans="1:4" ht="90.75" thickBot="1">
+    <row r="98" spans="1:4" ht="52" thickBot="1">
       <c r="A98" s="1" t="s">
         <v>292</v>
       </c>
@@ -4119,7 +4118,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="45.75" thickBot="1">
+    <row r="99" spans="1:4" ht="18" thickBot="1">
       <c r="A99" s="1" t="s">
         <v>295</v>
       </c>
@@ -4133,7 +4132,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="30.75" thickBot="1">
+    <row r="100" spans="1:4" ht="18" thickBot="1">
       <c r="A100" s="1" t="s">
         <v>298</v>
       </c>
@@ -4147,7 +4146,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="30.75" thickBot="1">
+    <row r="101" spans="1:4" ht="18" thickBot="1">
       <c r="A101" s="1" t="s">
         <v>301</v>
       </c>
@@ -4161,7 +4160,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="30.75" thickBot="1">
+    <row r="102" spans="1:4" ht="18" thickBot="1">
       <c r="A102" s="1" t="s">
         <v>304</v>
       </c>
@@ -4175,7 +4174,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="103" spans="1:4" ht="15.75" thickBot="1">
+    <row r="103" spans="1:4" ht="18" thickBot="1">
       <c r="A103" s="1" t="s">
         <v>307</v>
       </c>
@@ -4189,7 +4188,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="104" spans="1:4" ht="15.75" thickBot="1">
+    <row r="104" spans="1:4" ht="18" thickBot="1">
       <c r="A104" s="1" t="s">
         <v>310</v>
       </c>
@@ -4203,7 +4202,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="30.75" thickBot="1">
+    <row r="105" spans="1:4" ht="18" thickBot="1">
       <c r="A105" s="1" t="s">
         <v>313</v>
       </c>
@@ -4217,7 +4216,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="106" spans="1:4" ht="60.75" thickBot="1">
+    <row r="106" spans="1:4" ht="35" thickBot="1">
       <c r="A106" s="1" t="s">
         <v>316</v>
       </c>
@@ -4231,7 +4230,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="15.75" thickBot="1">
+    <row r="107" spans="1:4" ht="18" thickBot="1">
       <c r="A107" s="1" t="s">
         <v>319</v>
       </c>
@@ -4245,7 +4244,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="108" spans="1:4" ht="15.75" thickBot="1">
+    <row r="108" spans="1:4" ht="18" thickBot="1">
       <c r="A108" s="1" t="s">
         <v>322</v>
       </c>
@@ -4259,7 +4258,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="109" spans="1:4" ht="30.75" thickBot="1">
+    <row r="109" spans="1:4" ht="18" thickBot="1">
       <c r="A109" s="1" t="s">
         <v>325</v>
       </c>
@@ -4273,7 +4272,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="110" spans="1:4" ht="15.75" thickBot="1">
+    <row r="110" spans="1:4" ht="18" thickBot="1">
       <c r="A110" s="1" t="s">
         <v>328</v>
       </c>
@@ -4287,7 +4286,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="111" spans="1:4" ht="15.75" thickBot="1">
+    <row r="111" spans="1:4" ht="18" thickBot="1">
       <c r="A111" s="1" t="s">
         <v>331</v>
       </c>
@@ -4301,7 +4300,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="112" spans="1:4" ht="30.75" thickBot="1">
+    <row r="112" spans="1:4" ht="18" thickBot="1">
       <c r="A112" s="1" t="s">
         <v>334</v>
       </c>
@@ -4315,7 +4314,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="113" spans="1:4" ht="15.75" thickBot="1">
+    <row r="113" spans="1:4" ht="18" thickBot="1">
       <c r="A113" s="1" t="s">
         <v>337</v>
       </c>
@@ -4329,7 +4328,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="15.75" thickBot="1">
+    <row r="114" spans="1:4" ht="18" thickBot="1">
       <c r="A114" s="1" t="s">
         <v>340</v>
       </c>
@@ -4343,7 +4342,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="15.75" thickBot="1">
+    <row r="115" spans="1:4" ht="18" thickBot="1">
       <c r="A115" s="1" t="s">
         <v>343</v>
       </c>
@@ -4357,7 +4356,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="30.75" thickBot="1">
+    <row r="116" spans="1:4" ht="18" thickBot="1">
       <c r="A116" s="1" t="s">
         <v>346</v>
       </c>
@@ -4371,7 +4370,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="117" spans="1:4" ht="15.75" thickBot="1">
+    <row r="117" spans="1:4" ht="18" thickBot="1">
       <c r="A117" s="1" t="s">
         <v>349</v>
       </c>
@@ -4385,7 +4384,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="118" spans="1:4" ht="15.75" thickBot="1">
+    <row r="118" spans="1:4" ht="18" thickBot="1">
       <c r="A118" s="1" t="s">
         <v>352</v>
       </c>
@@ -4399,7 +4398,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="119" spans="1:4" ht="120.75" thickBot="1">
+    <row r="119" spans="1:4" ht="69" thickBot="1">
       <c r="A119" s="1" t="s">
         <v>355</v>
       </c>
@@ -4413,7 +4412,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="120" spans="1:4" ht="60.75" thickBot="1">
+    <row r="120" spans="1:4" ht="35" thickBot="1">
       <c r="A120" s="1" t="s">
         <v>358</v>
       </c>
@@ -4427,7 +4426,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="121" spans="1:4" ht="15.75" thickBot="1">
+    <row r="121" spans="1:4" ht="18" thickBot="1">
       <c r="A121" s="1" t="s">
         <v>361</v>
       </c>
@@ -4441,7 +4440,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="122" spans="1:4" ht="30.75" thickBot="1">
+    <row r="122" spans="1:4" ht="18" thickBot="1">
       <c r="A122" s="1" t="s">
         <v>364</v>
       </c>
@@ -4455,7 +4454,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="105.75" thickBot="1">
+    <row r="123" spans="1:4" ht="52" thickBot="1">
       <c r="A123" s="1" t="s">
         <v>367</v>
       </c>
@@ -4469,7 +4468,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="124" spans="1:4" ht="15.75" thickBot="1">
+    <row r="124" spans="1:4" ht="18" thickBot="1">
       <c r="A124" s="1" t="s">
         <v>370</v>
       </c>
@@ -4483,7 +4482,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="125" spans="1:4" ht="30.75" thickBot="1">
+    <row r="125" spans="1:4" ht="18" thickBot="1">
       <c r="A125" s="1" t="s">
         <v>373</v>
       </c>
@@ -4497,7 +4496,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="126" spans="1:4" ht="30.75" thickBot="1">
+    <row r="126" spans="1:4" ht="18" thickBot="1">
       <c r="A126" s="1" t="s">
         <v>376</v>
       </c>
@@ -4511,7 +4510,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="127" spans="1:4" ht="15.75" thickBot="1">
+    <row r="127" spans="1:4" ht="18" thickBot="1">
       <c r="A127" s="1" t="s">
         <v>379</v>
       </c>
@@ -4525,7 +4524,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="128" spans="1:4" ht="15.75" thickBot="1">
+    <row r="128" spans="1:4" ht="18" thickBot="1">
       <c r="A128" s="1" t="s">
         <v>382</v>
       </c>
@@ -4539,7 +4538,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="129" spans="1:4" ht="30.75" thickBot="1">
+    <row r="129" spans="1:4" ht="18" thickBot="1">
       <c r="A129" s="1" t="s">
         <v>385</v>
       </c>
@@ -4553,7 +4552,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="130" spans="1:4" ht="30.75" thickBot="1">
+    <row r="130" spans="1:4" ht="18" thickBot="1">
       <c r="A130" s="1" t="s">
         <v>388</v>
       </c>
@@ -4567,7 +4566,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="131" spans="1:4" ht="30.75" thickBot="1">
+    <row r="131" spans="1:4" ht="18" thickBot="1">
       <c r="A131" s="1" t="s">
         <v>391</v>
       </c>
@@ -4581,7 +4580,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="132" spans="1:4" ht="15.75" thickBot="1">
+    <row r="132" spans="1:4" ht="18" thickBot="1">
       <c r="A132" s="1" t="s">
         <v>394</v>
       </c>
@@ -4595,7 +4594,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="133" spans="1:4" ht="30.75" thickBot="1">
+    <row r="133" spans="1:4" ht="18" thickBot="1">
       <c r="A133" s="1" t="s">
         <v>397</v>
       </c>
@@ -4609,7 +4608,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="134" spans="1:4" ht="15.75" thickBot="1">
+    <row r="134" spans="1:4" ht="18" thickBot="1">
       <c r="A134" s="1" t="s">
         <v>400</v>
       </c>
@@ -4623,7 +4622,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="135" spans="1:4" ht="30.75" thickBot="1">
+    <row r="135" spans="1:4" ht="18" thickBot="1">
       <c r="A135" s="1" t="s">
         <v>403</v>
       </c>
@@ -4637,7 +4636,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="136" spans="1:4" ht="30.75" thickBot="1">
+    <row r="136" spans="1:4" ht="18" thickBot="1">
       <c r="A136" s="1" t="s">
         <v>406</v>
       </c>
@@ -4651,7 +4650,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="137" spans="1:4" ht="15.75" thickBot="1">
+    <row r="137" spans="1:4" ht="18" thickBot="1">
       <c r="A137" s="1" t="s">
         <v>409</v>
       </c>
@@ -4665,7 +4664,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="138" spans="1:4" ht="15.75" thickBot="1">
+    <row r="138" spans="1:4" ht="18" thickBot="1">
       <c r="A138" s="1" t="s">
         <v>412</v>
       </c>
@@ -4679,7 +4678,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="139" spans="1:4" ht="45.75" thickBot="1">
+    <row r="139" spans="1:4" ht="35" thickBot="1">
       <c r="A139" s="1" t="s">
         <v>415</v>
       </c>
@@ -4693,7 +4692,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="140" spans="1:4" ht="30.75" thickBot="1">
+    <row r="140" spans="1:4" ht="18" thickBot="1">
       <c r="A140" s="1" t="s">
         <v>418</v>
       </c>
@@ -4707,7 +4706,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="141" spans="1:4" ht="30.75" thickBot="1">
+    <row r="141" spans="1:4" ht="18" thickBot="1">
       <c r="A141" s="1" t="s">
         <v>421</v>
       </c>
@@ -4721,7 +4720,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="142" spans="1:4" ht="30.75" thickBot="1">
+    <row r="142" spans="1:4" ht="18" thickBot="1">
       <c r="A142" s="1" t="s">
         <v>424</v>
       </c>
@@ -4735,7 +4734,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="143" spans="1:4" ht="15.75" thickBot="1">
+    <row r="143" spans="1:4" ht="18" thickBot="1">
       <c r="A143" s="1" t="s">
         <v>427</v>
       </c>
@@ -4749,7 +4748,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="144" spans="1:4" ht="15.75" thickBot="1">
+    <row r="144" spans="1:4" ht="18" thickBot="1">
       <c r="A144" s="1" t="s">
         <v>430</v>
       </c>
@@ -4763,7 +4762,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="145" spans="1:4" ht="90.75" thickBot="1">
+    <row r="145" spans="1:4" ht="52" thickBot="1">
       <c r="A145" s="1" t="s">
         <v>433</v>
       </c>
@@ -4777,7 +4776,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="146" spans="1:4" ht="60.75" thickBot="1">
+    <row r="146" spans="1:4" ht="35" thickBot="1">
       <c r="A146" s="1" t="s">
         <v>436</v>
       </c>
@@ -4791,7 +4790,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="147" spans="1:4" ht="30.75" thickBot="1">
+    <row r="147" spans="1:4" ht="18" thickBot="1">
       <c r="A147" s="1" t="s">
         <v>439</v>
       </c>
@@ -4805,7 +4804,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="148" spans="1:4" ht="30.75" thickBot="1">
+    <row r="148" spans="1:4" ht="18" thickBot="1">
       <c r="A148" s="1" t="s">
         <v>442</v>
       </c>
@@ -4819,7 +4818,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="149" spans="1:4" ht="30.75" thickBot="1">
+    <row r="149" spans="1:4" ht="18" thickBot="1">
       <c r="A149" s="1" t="s">
         <v>445</v>
       </c>
@@ -4833,7 +4832,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="150" spans="1:4" ht="30.75" thickBot="1">
+    <row r="150" spans="1:4" ht="18" thickBot="1">
       <c r="A150" s="1" t="s">
         <v>448</v>
       </c>
@@ -4847,7 +4846,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="151" spans="1:4" ht="30.75" thickBot="1">
+    <row r="151" spans="1:4" ht="18" thickBot="1">
       <c r="A151" s="1" t="s">
         <v>451</v>
       </c>
@@ -4861,7 +4860,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="152" spans="1:4" ht="30.75" thickBot="1">
+    <row r="152" spans="1:4" ht="18" thickBot="1">
       <c r="A152" s="1" t="s">
         <v>454</v>
       </c>
@@ -4875,7 +4874,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="153" spans="1:4" ht="30.75" thickBot="1">
+    <row r="153" spans="1:4" ht="18" thickBot="1">
       <c r="A153" s="1" t="s">
         <v>457</v>
       </c>
@@ -4889,7 +4888,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="154" spans="1:4" ht="30.75" thickBot="1">
+    <row r="154" spans="1:4" ht="18" thickBot="1">
       <c r="A154" s="1" t="s">
         <v>460</v>
       </c>
@@ -4903,7 +4902,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="155" spans="1:4" ht="15.75" thickBot="1">
+    <row r="155" spans="1:4" ht="18" thickBot="1">
       <c r="A155" s="1" t="s">
         <v>463</v>
       </c>
@@ -4917,7 +4916,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="156" spans="1:4" ht="15.75" thickBot="1">
+    <row r="156" spans="1:4" ht="18" thickBot="1">
       <c r="A156" s="1" t="s">
         <v>466</v>
       </c>
@@ -4931,7 +4930,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="157" spans="1:4" ht="45.75" thickBot="1">
+    <row r="157" spans="1:4" ht="18" thickBot="1">
       <c r="A157" s="1" t="s">
         <v>469</v>
       </c>
@@ -4945,7 +4944,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="158" spans="1:4" ht="45.75" thickBot="1">
+    <row r="158" spans="1:4" ht="18" thickBot="1">
       <c r="A158" s="1" t="s">
         <v>472</v>
       </c>
@@ -4959,7 +4958,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="159" spans="1:4" ht="45.75" thickBot="1">
+    <row r="159" spans="1:4" ht="18" thickBot="1">
       <c r="A159" s="1" t="s">
         <v>475</v>
       </c>
@@ -4973,7 +4972,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="160" spans="1:4" ht="30.75" thickBot="1">
+    <row r="160" spans="1:4" ht="18" thickBot="1">
       <c r="A160" s="1" t="s">
         <v>478</v>
       </c>
@@ -4987,7 +4986,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="161" spans="1:4" ht="30.75" thickBot="1">
+    <row r="161" spans="1:4" ht="18" thickBot="1">
       <c r="A161" s="1" t="s">
         <v>481</v>
       </c>
@@ -5001,7 +5000,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="162" spans="1:4" ht="15.75" thickBot="1">
+    <row r="162" spans="1:4" ht="18" thickBot="1">
       <c r="A162" s="1" t="s">
         <v>484</v>
       </c>
@@ -5015,7 +5014,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="163" spans="1:4" ht="15.75" thickBot="1">
+    <row r="163" spans="1:4" ht="18" thickBot="1">
       <c r="A163" s="1" t="s">
         <v>487</v>
       </c>
@@ -5029,7 +5028,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="164" spans="1:4" ht="30.75" thickBot="1">
+    <row r="164" spans="1:4" ht="18" thickBot="1">
       <c r="A164" s="1" t="s">
         <v>490</v>
       </c>
@@ -5043,7 +5042,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="165" spans="1:4" ht="90.75" thickBot="1">
+    <row r="165" spans="1:4" ht="35" thickBot="1">
       <c r="A165" s="1" t="s">
         <v>493</v>
       </c>
@@ -5057,7 +5056,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="166" spans="1:4" ht="15.75" thickBot="1">
+    <row r="166" spans="1:4" ht="18" thickBot="1">
       <c r="A166" s="1" t="s">
         <v>496</v>
       </c>
@@ -5071,7 +5070,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="167" spans="1:4" ht="15.75" thickBot="1">
+    <row r="167" spans="1:4" ht="18" thickBot="1">
       <c r="A167" s="1" t="s">
         <v>499</v>
       </c>
@@ -5085,7 +5084,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="168" spans="1:4" ht="30.75" thickBot="1">
+    <row r="168" spans="1:4" ht="18" thickBot="1">
       <c r="A168" s="1" t="s">
         <v>502</v>
       </c>
@@ -5099,7 +5098,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="169" spans="1:4" ht="15.75" thickBot="1">
+    <row r="169" spans="1:4" ht="18" thickBot="1">
       <c r="A169" s="1" t="s">
         <v>505</v>
       </c>
@@ -5113,7 +5112,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="170" spans="1:4" ht="45.75" thickBot="1">
+    <row r="170" spans="1:4" ht="35" thickBot="1">
       <c r="A170" s="1" t="s">
         <v>508</v>
       </c>
@@ -5127,7 +5126,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="171" spans="1:4" ht="30.75" thickBot="1">
+    <row r="171" spans="1:4" ht="18" thickBot="1">
       <c r="A171" s="1" t="s">
         <v>511</v>
       </c>
@@ -5141,7 +5140,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="172" spans="1:4" ht="45.75" thickBot="1">
+    <row r="172" spans="1:4" ht="35" thickBot="1">
       <c r="A172" s="1" t="s">
         <v>514</v>
       </c>
@@ -5155,7 +5154,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="173" spans="1:4" ht="30.75" thickBot="1">
+    <row r="173" spans="1:4" ht="18" thickBot="1">
       <c r="A173" s="1" t="s">
         <v>517</v>
       </c>
@@ -5169,7 +5168,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="174" spans="1:4" ht="15.75" thickBot="1">
+    <row r="174" spans="1:4" ht="18" thickBot="1">
       <c r="A174" s="1" t="s">
         <v>520</v>
       </c>
@@ -5183,7 +5182,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="175" spans="1:4" ht="45.75" thickBot="1">
+    <row r="175" spans="1:4" ht="18" thickBot="1">
       <c r="A175" s="1" t="s">
         <v>523</v>
       </c>
@@ -5197,7 +5196,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="176" spans="1:4" ht="15.75" thickBot="1">
+    <row r="176" spans="1:4" ht="18" thickBot="1">
       <c r="A176" s="1" t="s">
         <v>526</v>
       </c>
@@ -5211,7 +5210,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="177" spans="1:4" ht="15.75" thickBot="1">
+    <row r="177" spans="1:4" ht="18" thickBot="1">
       <c r="A177" s="1" t="s">
         <v>529</v>
       </c>
@@ -5225,7 +5224,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="178" spans="1:4" ht="30.75" thickBot="1">
+    <row r="178" spans="1:4" ht="18" thickBot="1">
       <c r="A178" s="1" t="s">
         <v>532</v>
       </c>
@@ -5239,7 +5238,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="179" spans="1:4" ht="30.75" thickBot="1">
+    <row r="179" spans="1:4" ht="18" thickBot="1">
       <c r="A179" s="1" t="s">
         <v>535</v>
       </c>
@@ -5253,7 +5252,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="180" spans="1:4" ht="15.75" thickBot="1">
+    <row r="180" spans="1:4" ht="18" thickBot="1">
       <c r="A180" s="1" t="s">
         <v>538</v>
       </c>
@@ -5267,7 +5266,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="181" spans="1:4" ht="75.75" thickBot="1">
+    <row r="181" spans="1:4" ht="35" thickBot="1">
       <c r="A181" s="1" t="s">
         <v>541</v>
       </c>
@@ -5281,7 +5280,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="182" spans="1:4" ht="30.75" thickBot="1">
+    <row r="182" spans="1:4" ht="18" thickBot="1">
       <c r="A182" s="1" t="s">
         <v>544</v>
       </c>
@@ -5295,7 +5294,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="183" spans="1:4" ht="75.75" thickBot="1">
+    <row r="183" spans="1:4" ht="35" thickBot="1">
       <c r="A183" s="1" t="s">
         <v>547</v>
       </c>
@@ -5309,7 +5308,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="184" spans="1:4" ht="30.75" thickBot="1">
+    <row r="184" spans="1:4" ht="18" thickBot="1">
       <c r="A184" s="1" t="s">
         <v>550</v>
       </c>
@@ -5323,7 +5322,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="185" spans="1:4" ht="30.75" thickBot="1">
+    <row r="185" spans="1:4" ht="18" thickBot="1">
       <c r="A185" s="1" t="s">
         <v>553</v>
       </c>
@@ -5337,7 +5336,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="186" spans="1:4" ht="45.75" thickBot="1">
+    <row r="186" spans="1:4" ht="18" thickBot="1">
       <c r="A186" s="1" t="s">
         <v>556</v>
       </c>
@@ -5351,7 +5350,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="187" spans="1:4" ht="105.75" thickBot="1">
+    <row r="187" spans="1:4" ht="52" thickBot="1">
       <c r="A187" s="1" t="s">
         <v>559</v>
       </c>
@@ -5365,7 +5364,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="188" spans="1:4" ht="60.75" thickBot="1">
+    <row r="188" spans="1:4" ht="35" thickBot="1">
       <c r="A188" s="1" t="s">
         <v>562</v>
       </c>
@@ -5379,7 +5378,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="189" spans="1:4" ht="30.75" thickBot="1">
+    <row r="189" spans="1:4" ht="18" thickBot="1">
       <c r="A189" s="1" t="s">
         <v>565</v>
       </c>
@@ -5393,7 +5392,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="190" spans="1:4" ht="60.75" thickBot="1">
+    <row r="190" spans="1:4" ht="35" thickBot="1">
       <c r="A190" s="1" t="s">
         <v>568</v>
       </c>
@@ -5407,7 +5406,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="191" spans="1:4" ht="75.75" thickBot="1">
+    <row r="191" spans="1:4" ht="35" thickBot="1">
       <c r="A191" s="1" t="s">
         <v>571</v>
       </c>
@@ -5421,7 +5420,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="192" spans="1:4" ht="75.75" thickBot="1">
+    <row r="192" spans="1:4" ht="35" thickBot="1">
       <c r="A192" s="1" t="s">
         <v>574</v>
       </c>
@@ -5435,7 +5434,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="193" spans="1:4" ht="15.75" thickBot="1">
+    <row r="193" spans="1:4" ht="18" thickBot="1">
       <c r="A193" s="1" t="s">
         <v>577</v>
       </c>
@@ -5449,7 +5448,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="194" spans="1:4" ht="30.75" thickBot="1">
+    <row r="194" spans="1:4" ht="18" thickBot="1">
       <c r="A194" s="1" t="s">
         <v>580</v>
       </c>
@@ -5463,7 +5462,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="195" spans="1:4" ht="75.75" thickBot="1">
+    <row r="195" spans="1:4" ht="35" thickBot="1">
       <c r="A195" s="1" t="s">
         <v>583</v>
       </c>
@@ -5477,7 +5476,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="196" spans="1:4" ht="30.75" thickBot="1">
+    <row r="196" spans="1:4" ht="18" thickBot="1">
       <c r="A196" s="1" t="s">
         <v>586</v>
       </c>
@@ -5491,7 +5490,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="197" spans="1:4" ht="30.75" thickBot="1">
+    <row r="197" spans="1:4" ht="18" thickBot="1">
       <c r="A197" s="1" t="s">
         <v>589</v>
       </c>
@@ -5505,7 +5504,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="198" spans="1:4" ht="15.75" thickBot="1">
+    <row r="198" spans="1:4" ht="18" thickBot="1">
       <c r="A198" s="1" t="s">
         <v>592</v>
       </c>
@@ -5519,7 +5518,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="199" spans="1:4" ht="30.75" thickBot="1">
+    <row r="199" spans="1:4" ht="18" thickBot="1">
       <c r="A199" s="1" t="s">
         <v>595</v>
       </c>
@@ -5533,7 +5532,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="200" spans="1:4" ht="30.75" thickBot="1">
+    <row r="200" spans="1:4" ht="18" thickBot="1">
       <c r="A200" s="1" t="s">
         <v>598</v>
       </c>
@@ -5547,7 +5546,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="201" spans="1:4" ht="30.75" thickBot="1">
+    <row r="201" spans="1:4" ht="18" thickBot="1">
       <c r="A201" s="1" t="s">
         <v>601</v>
       </c>
@@ -5561,7 +5560,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="202" spans="1:4" ht="75.75" thickBot="1">
+    <row r="202" spans="1:4" ht="35" thickBot="1">
       <c r="A202" s="1" t="s">
         <v>604</v>
       </c>
@@ -5575,7 +5574,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="203" spans="1:4" ht="30.75" thickBot="1">
+    <row r="203" spans="1:4" ht="18" thickBot="1">
       <c r="A203" s="1" t="s">
         <v>607</v>
       </c>
@@ -5589,7 +5588,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="204" spans="1:4" ht="30.75" thickBot="1">
+    <row r="204" spans="1:4" ht="18" thickBot="1">
       <c r="A204" s="1" t="s">
         <v>610</v>
       </c>
@@ -5603,7 +5602,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="205" spans="1:4" ht="45.75" thickBot="1">
+    <row r="205" spans="1:4" ht="18" thickBot="1">
       <c r="A205" s="1" t="s">
         <v>613</v>
       </c>
@@ -5617,7 +5616,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="206" spans="1:4" ht="30.75" thickBot="1">
+    <row r="206" spans="1:4" ht="18" thickBot="1">
       <c r="A206" s="1" t="s">
         <v>616</v>
       </c>
@@ -5631,7 +5630,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="207" spans="1:4" ht="30.75" thickBot="1">
+    <row r="207" spans="1:4" ht="18" thickBot="1">
       <c r="A207" s="1" t="s">
         <v>619</v>
       </c>
@@ -5645,7 +5644,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="208" spans="1:4" ht="120.75" thickBot="1">
+    <row r="208" spans="1:4" ht="52" thickBot="1">
       <c r="A208" s="1" t="s">
         <v>622</v>
       </c>
@@ -5659,7 +5658,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="209" spans="1:4" ht="30.75" thickBot="1">
+    <row r="209" spans="1:4" ht="18" thickBot="1">
       <c r="A209" s="1" t="s">
         <v>625</v>
       </c>
@@ -5673,7 +5672,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="210" spans="1:4" ht="15.75" thickBot="1">
+    <row r="210" spans="1:4" ht="18" thickBot="1">
       <c r="A210" s="1" t="s">
         <v>628</v>
       </c>
@@ -5687,7 +5686,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="211" spans="1:4" ht="30.75" thickBot="1">
+    <row r="211" spans="1:4" ht="18" thickBot="1">
       <c r="A211" s="1" t="s">
         <v>631</v>
       </c>
@@ -5701,7 +5700,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="212" spans="1:4" ht="30.75" thickBot="1">
+    <row r="212" spans="1:4" ht="18" thickBot="1">
       <c r="A212" s="1" t="s">
         <v>634</v>
       </c>
@@ -5715,7 +5714,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="213" spans="1:4" ht="30.75" thickBot="1">
+    <row r="213" spans="1:4" ht="18" thickBot="1">
       <c r="A213" s="1" t="s">
         <v>637</v>
       </c>
@@ -5729,7 +5728,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="214" spans="1:4" ht="60.75" thickBot="1">
+    <row r="214" spans="1:4" ht="35" thickBot="1">
       <c r="A214" s="1" t="s">
         <v>640</v>
       </c>
@@ -5743,7 +5742,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="215" spans="1:4" ht="30.75" thickBot="1">
+    <row r="215" spans="1:4" ht="18" thickBot="1">
       <c r="A215" s="1" t="s">
         <v>643</v>
       </c>
@@ -5757,7 +5756,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="216" spans="1:4" ht="30.75" thickBot="1">
+    <row r="216" spans="1:4" ht="18" thickBot="1">
       <c r="A216" s="1" t="s">
         <v>646</v>
       </c>
@@ -5771,7 +5770,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="217" spans="1:4" ht="60.75" thickBot="1">
+    <row r="217" spans="1:4" ht="35" thickBot="1">
       <c r="A217" s="1" t="s">
         <v>649</v>
       </c>
@@ -5785,7 +5784,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="218" spans="1:4" ht="60.75" thickBot="1">
+    <row r="218" spans="1:4" ht="35" thickBot="1">
       <c r="A218" s="1" t="s">
         <v>652</v>
       </c>
@@ -5799,7 +5798,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="219" spans="1:4" ht="30.75" thickBot="1">
+    <row r="219" spans="1:4" ht="18" thickBot="1">
       <c r="A219" s="1" t="s">
         <v>655</v>
       </c>
@@ -5813,7 +5812,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="220" spans="1:4" ht="75.75" thickBot="1">
+    <row r="220" spans="1:4" ht="35" thickBot="1">
       <c r="A220" s="1" t="s">
         <v>658</v>
       </c>
@@ -5827,7 +5826,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="221" spans="1:4" ht="30.75" thickBot="1">
+    <row r="221" spans="1:4" ht="18" thickBot="1">
       <c r="A221" s="1" t="s">
         <v>661</v>
       </c>
@@ -5841,7 +5840,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="222" spans="1:4" ht="30.75" thickBot="1">
+    <row r="222" spans="1:4" ht="18" thickBot="1">
       <c r="A222" s="1" t="s">
         <v>664</v>
       </c>
@@ -5855,7 +5854,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="223" spans="1:4" ht="15.75" thickBot="1">
+    <row r="223" spans="1:4" ht="18" thickBot="1">
       <c r="A223" s="1" t="s">
         <v>667</v>
       </c>
@@ -5869,7 +5868,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="224" spans="1:4" ht="15.75" thickBot="1">
+    <row r="224" spans="1:4" ht="18" thickBot="1">
       <c r="A224" s="1" t="s">
         <v>670</v>
       </c>
@@ -5883,7 +5882,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="225" spans="1:4" ht="15.75" thickBot="1">
+    <row r="225" spans="1:4" ht="18" thickBot="1">
       <c r="A225" s="1" t="s">
         <v>673</v>
       </c>
@@ -5897,7 +5896,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="226" spans="1:4" ht="45.75" thickBot="1">
+    <row r="226" spans="1:4" ht="35" thickBot="1">
       <c r="A226" s="1" t="s">
         <v>676</v>
       </c>
@@ -5911,7 +5910,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="227" spans="1:4" ht="15.75" thickBot="1">
+    <row r="227" spans="1:4" ht="18" thickBot="1">
       <c r="A227" s="1" t="s">
         <v>679</v>
       </c>
@@ -5925,7 +5924,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="228" spans="1:4" ht="15.75" thickBot="1">
+    <row r="228" spans="1:4" ht="18" thickBot="1">
       <c r="A228" s="1" t="s">
         <v>682</v>
       </c>
@@ -5939,7 +5938,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="229" spans="1:4" ht="30.75" thickBot="1">
+    <row r="229" spans="1:4" ht="18" thickBot="1">
       <c r="A229" s="1" t="s">
         <v>685</v>
       </c>
@@ -5953,7 +5952,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="230" spans="1:4" ht="75.75" thickBot="1">
+    <row r="230" spans="1:4" ht="35" thickBot="1">
       <c r="A230" s="1" t="s">
         <v>688</v>
       </c>
@@ -5967,7 +5966,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="231" spans="1:4" ht="15.75" thickBot="1">
+    <row r="231" spans="1:4" ht="18" thickBot="1">
       <c r="A231" s="1" t="s">
         <v>691</v>
       </c>
@@ -5981,7 +5980,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="232" spans="1:4" ht="15.75" thickBot="1">
+    <row r="232" spans="1:4" ht="18" thickBot="1">
       <c r="A232" s="1" t="s">
         <v>694</v>
       </c>
@@ -5995,7 +5994,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="233" spans="1:4" ht="15.75" thickBot="1">
+    <row r="233" spans="1:4" ht="18" thickBot="1">
       <c r="A233" s="1" t="s">
         <v>697</v>
       </c>
@@ -6009,7 +6008,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="234" spans="1:4" ht="60.75" thickBot="1">
+    <row r="234" spans="1:4" ht="35" thickBot="1">
       <c r="A234" s="1" t="s">
         <v>700</v>
       </c>
@@ -6023,7 +6022,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="235" spans="1:4" ht="150.75" thickBot="1">
+    <row r="235" spans="1:4" ht="69" thickBot="1">
       <c r="A235" s="1" t="s">
         <v>703</v>
       </c>
@@ -6037,7 +6036,7 @@
         <v>826</v>
       </c>
     </row>
-    <row r="236" spans="1:4" ht="90.75" thickBot="1">
+    <row r="236" spans="1:4" ht="52" thickBot="1">
       <c r="A236" s="1" t="s">
         <v>706</v>
       </c>
@@ -6051,7 +6050,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="237" spans="1:4" ht="75.75" thickBot="1">
+    <row r="237" spans="1:4" ht="35" thickBot="1">
       <c r="A237" s="1" t="s">
         <v>709</v>
       </c>
@@ -6065,7 +6064,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="238" spans="1:4" ht="30.75" thickBot="1">
+    <row r="238" spans="1:4" ht="18" thickBot="1">
       <c r="A238" s="1" t="s">
         <v>712</v>
       </c>
@@ -6079,7 +6078,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="239" spans="1:4" ht="30.75" thickBot="1">
+    <row r="239" spans="1:4" ht="18" thickBot="1">
       <c r="A239" s="1" t="s">
         <v>715</v>
       </c>
@@ -6093,7 +6092,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="240" spans="1:4" ht="30.75" thickBot="1">
+    <row r="240" spans="1:4" ht="18" thickBot="1">
       <c r="A240" s="1" t="s">
         <v>718</v>
       </c>
@@ -6107,7 +6106,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="241" spans="1:4" ht="90.75" thickBot="1">
+    <row r="241" spans="1:4" ht="52" thickBot="1">
       <c r="A241" s="1" t="s">
         <v>721</v>
       </c>
@@ -6121,7 +6120,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="242" spans="1:4" ht="30.75" thickBot="1">
+    <row r="242" spans="1:4" ht="18" thickBot="1">
       <c r="A242" s="1" t="s">
         <v>724</v>
       </c>
@@ -6135,7 +6134,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="243" spans="1:4" ht="45.75" thickBot="1">
+    <row r="243" spans="1:4" ht="35" thickBot="1">
       <c r="A243" s="1" t="s">
         <v>727</v>
       </c>
@@ -6149,7 +6148,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="244" spans="1:4" ht="45.75" thickBot="1">
+    <row r="244" spans="1:4" ht="35" thickBot="1">
       <c r="A244" s="1" t="s">
         <v>730</v>
       </c>
@@ -6163,7 +6162,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="245" spans="1:4" ht="45.75" thickBot="1">
+    <row r="245" spans="1:4" ht="35" thickBot="1">
       <c r="A245" s="1" t="s">
         <v>733</v>
       </c>
@@ -6177,7 +6176,7 @@
         <v>876</v>
       </c>
     </row>
-    <row r="246" spans="1:4" ht="45.75" thickBot="1">
+    <row r="246" spans="1:4" ht="18" thickBot="1">
       <c r="A246" s="1" t="s">
         <v>736</v>
       </c>
@@ -6191,7 +6190,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="247" spans="1:4" ht="15.75" thickBot="1">
+    <row r="247" spans="1:4" ht="18" thickBot="1">
       <c r="A247" s="1" t="s">
         <v>739</v>
       </c>
@@ -6205,7 +6204,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="248" spans="1:4" ht="15.75" thickBot="1">
+    <row r="248" spans="1:4" ht="18" thickBot="1">
       <c r="A248" s="1" t="s">
         <v>742</v>
       </c>
@@ -6219,7 +6218,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="249" spans="1:4" ht="30.75" thickBot="1">
+    <row r="249" spans="1:4" ht="18" thickBot="1">
       <c r="A249" s="1" t="s">
         <v>745</v>
       </c>
@@ -6233,7 +6232,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="250" spans="1:4" ht="30.75" thickBot="1">
+    <row r="250" spans="1:4" ht="18" thickBot="1">
       <c r="A250" s="1" t="s">
         <v>748</v>
       </c>

</xml_diff>